<commit_message>
hoja de descarga de consulta incial
</commit_message>
<xml_diff>
--- a/src/main/resources/Template-Historia.xlsx
+++ b/src/main/resources/Template-Historia.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gastón\Documents\GitHub\SGHM-API\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9059C848-6B89-4D0F-AE33-A701FC8EFF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A933C9B-6C86-4394-8599-BB864E415ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A2D828E-F264-40FB-9DBB-6B51D59DB6F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5A2D828E-F264-40FB-9DBB-6B51D59DB6F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Personales" sheetId="1" r:id="rId1"/>
+    <sheet name="Consulta Inicial" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Datos personales del paciente</t>
   </si>
@@ -93,6 +94,42 @@
   </si>
   <si>
     <t>Sin alteraciones craneales, como si fuera cesárea</t>
+  </si>
+  <si>
+    <t>Consulta incial del paciente</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Fecha de Consulta</t>
+  </si>
+  <si>
+    <t>Actividad Física</t>
+  </si>
+  <si>
+    <t>Antigüedad</t>
+  </si>
+  <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>Intensidad</t>
+  </si>
+  <si>
+    <t>Característica</t>
+  </si>
+  <si>
+    <t>Irradiación</t>
+  </si>
+  <si>
+    <t>Atenua</t>
+  </si>
+  <si>
+    <t>Covid</t>
+  </si>
+  <si>
+    <t>Fecha de Covid</t>
   </si>
 </sst>
 </file>
@@ -124,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +174,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -257,45 +300,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -310,9 +329,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -320,9 +344,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,147 +748,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93810E7-F0A5-427D-BD47-810E66C61BB7}">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="8">
         <v>39222</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B2:F4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B15:C15"/>
@@ -801,13 +910,199 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B2:F4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74A42A0-BFD1-4741-B885-362106670526}">
+  <dimension ref="B1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="37">
+        <v>39222</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="44"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="44"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="44"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="B2:F4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hoja de antecedentes en descarga
</commit_message>
<xml_diff>
--- a/src/main/resources/Template-Historia.xlsx
+++ b/src/main/resources/Template-Historia.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gastón\Documents\GitHub\SGHM-API\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A933C9B-6C86-4394-8599-BB864E415ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572A745F-AA47-4A63-AB41-2CD17CF7AEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5A2D828E-F264-40FB-9DBB-6B51D59DB6F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{5A2D828E-F264-40FB-9DBB-6B51D59DB6F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Personales" sheetId="1" r:id="rId1"/>
     <sheet name="Consulta Inicial" sheetId="2" r:id="rId2"/>
+    <sheet name="Antecedentes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
   <si>
     <t>Datos personales del paciente</t>
   </si>
@@ -130,13 +131,121 @@
   </si>
   <si>
     <t>Fecha de Covid</t>
+  </si>
+  <si>
+    <t>Cirugías</t>
+  </si>
+  <si>
+    <t>Odontología</t>
+  </si>
+  <si>
+    <t>Implantes superiores</t>
+  </si>
+  <si>
+    <t>Implantes inferiores</t>
+  </si>
+  <si>
+    <t>Piezas faltantes superiores</t>
+  </si>
+  <si>
+    <t>Piezas faltantes inferiores</t>
+  </si>
+  <si>
+    <t>Prótesis</t>
+  </si>
+  <si>
+    <t>Placa de contención</t>
+  </si>
+  <si>
+    <t>Placa de descanso</t>
+  </si>
+  <si>
+    <t>Ortodoncia</t>
+  </si>
+  <si>
+    <t>Edad ortodoncia</t>
+  </si>
+  <si>
+    <t>Salud femenina</t>
+  </si>
+  <si>
+    <t>Menstruación</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>Duración</t>
+  </si>
+  <si>
+    <t>Volúmen</t>
+  </si>
+  <si>
+    <t>Embarazos</t>
+  </si>
+  <si>
+    <t>Partos/Cesáreas</t>
+  </si>
+  <si>
+    <t>Abortos espontáneos</t>
+  </si>
+  <si>
+    <t>Abortos inducidos</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
+  </si>
+  <si>
+    <t>Intestinal</t>
+  </si>
+  <si>
+    <t>Digestivo</t>
+  </si>
+  <si>
+    <t>Cardíaco</t>
+  </si>
+  <si>
+    <t>Urogenital</t>
+  </si>
+  <si>
+    <t>Óseo</t>
+  </si>
+  <si>
+    <t>Fuma</t>
+  </si>
+  <si>
+    <t>Otras drogas</t>
+  </si>
+  <si>
+    <t>Accidentes</t>
+  </si>
+  <si>
+    <t>Medicación</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Fracturas</t>
+  </si>
+  <si>
+    <t>Tiroides</t>
+  </si>
+  <si>
+    <t>Dolores de cabeza</t>
+  </si>
+  <si>
+    <t>Pérdidas</t>
+  </si>
+  <si>
+    <t>Alimentación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +269,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +297,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -309,12 +432,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -329,10 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -344,88 +552,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,144 +999,139 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="15">
         <v>39222</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B2:F4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B15:C15"/>
@@ -910,6 +1148,11 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:F4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -920,171 +1163,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74A42A0-BFD1-4741-B885-362106670526}">
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="33">
         <v>39222</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="44"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="44"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
     </row>
     <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B2:F4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="B14:C14"/>
@@ -1095,13 +1339,540 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:F12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B15:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21645043-914D-4E3A-97F4-86D9941A7D96}">
+  <dimension ref="B1:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="71"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="68"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+    </row>
+    <row r="9" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="71"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="57">
+        <v>39222</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="71"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="57">
+        <v>39222</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="71"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="57">
+        <v>39222</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="71"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="26"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="57">
+        <v>39222</v>
+      </c>
+      <c r="D42" s="16"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="59"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="31"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="18"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="73">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="B2:F4"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>